<commit_message>
remove h call brutes
</commit_message>
<xml_diff>
--- a/python things/final_project.xlsx
+++ b/python things/final_project.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epflch-my.sharepoint.com/personal/carlos_colladocapell_epfl_ch/Documents/Fall 2023/MATH-454 Parallel and high-performance computing/GitLab/final_project/python things/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00996E35-032C-AC46-BD88-FC0EA127BD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{00996E35-032C-AC46-BD88-FC0EA127BD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EFD9D22-6B5A-DB40-9DC5-FF88D263C3B5}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16840" xr2:uid="{A85BE527-750F-D341-B4BA-EA0C8FBBE84B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Profiling" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,15 +35,86 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+  <si>
+    <t>% Time</t>
+  </si>
+  <si>
+    <t>Cumulative Seconds</t>
+  </si>
+  <si>
+    <t>Self Seconds</t>
+  </si>
+  <si>
+    <t>Calls</t>
+  </si>
+  <si>
+    <t>Self s/call</t>
+  </si>
+  <si>
+    <t>Total s/call</t>
+  </si>
+  <si>
+    <t>Function Name</t>
+  </si>
+  <si>
+    <t>compute_brute_force</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>update_positions</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>get_nbr_particles</t>
+  </si>
+  <si>
+    <t>nbodybruteforce</t>
+  </si>
+  <si>
+    <t>print_parameters</t>
+  </si>
+  <si>
+    <t>read_test_case</t>
+  </si>
+  <si>
+    <t>brute force</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF374151"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF374151"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,8 +137,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,12 +456,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7AF904-0670-B64A-BE6F-B666A3BE6420}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="181" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>89.06</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3.78</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.78</v>
+      </c>
+      <c r="D4" s="3">
+        <v>40000</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>8.73</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4.16</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="D5" s="3">
+        <v>376713688</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>1.18</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4.21</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4.21</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4.21</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4.21</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4.21</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4.16</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4.21</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4.21</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new loc of if clause mpi
</commit_message>
<xml_diff>
--- a/python things/final_project.xlsx
+++ b/python things/final_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epflch-my.sharepoint.com/personal/carlos_colladocapell_epfl_ch/Documents/Fall 2023/MATH-454 Parallel and high-performance computing/GitLab/final_project/python things/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{00996E35-032C-AC46-BD88-FC0EA127BD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14B4B834-5DC9-A94F-9A04-2FCFAD03375C}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="8_{00996E35-032C-AC46-BD88-FC0EA127BD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01C80789-08E0-474B-AF38-83DBBF4E31AB}"/>
   <bookViews>
     <workbookView xWindow="14540" yWindow="7280" windowWidth="14860" windowHeight="10240" xr2:uid="{A85BE527-750F-D341-B4BA-EA0C8FBBE84B}"/>
   </bookViews>
@@ -392,13 +392,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7AF904-0670-B64A-BE6F-B666A3BE6420}">
   <dimension ref="A2:AA134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3712,12 +3713,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>36</v>
       </c>
@@ -3725,22 +3726,29 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>42</v>
       </c>
@@ -3748,17 +3756,17 @@
         <v>85</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>88</v>
       </c>

</xml_diff>